<commit_message>
Revised 2015 data and results
</commit_message>
<xml_diff>
--- a/FieldData/2015/xlsx_analysis/01-003-B Field Data.xlsx
+++ b/FieldData/2015/xlsx_analysis/01-003-B Field Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fc4fc14c9be0aac/Documents/GitHub/CompSites/FieldData/2015/xlsx_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_02EB18C22B45611C0549717AD63E65C13BF7C481" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C35F5DF6-76EB-4E96-86C9-B3F2E4B15598}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_02EB18C22B45611C0549717AD63E65C13BF7C481" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AF7AA4D-70E4-497E-A2E2-CB5B001ABF8D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="83">
   <si>
     <t>PLOT</t>
   </si>
   <si>
     <t>COMMUNITY</t>
-  </si>
-  <si>
-    <t>Common</t>
   </si>
   <si>
     <t>Scientific</t>
@@ -268,9 +265,6 @@
     <t>common spike-rush</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>western St. John's-wort</t>
   </si>
   <si>
@@ -293,9 +287,6 @@
     <t>U</t>
   </si>
   <si>
-    <t>Percent_Cover</t>
-  </si>
-  <si>
     <t>SITE_ID</t>
   </si>
   <si>
@@ -303,6 +294,15 @@
   </si>
   <si>
     <t>ORIGIN</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>SPECIES_CODE</t>
+  </si>
+  <si>
+    <t>PERCENT_COVER</t>
   </si>
 </sst>
 </file>
@@ -877,7 +877,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -928,14 +928,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="145">
@@ -2414,8 +2423,8 @@
   <dimension ref="A1:IN107"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2433,7 +2442,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -2442,113 +2451,111 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>2</v>
+        <v>81</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>82</v>
-      </c>
       <c r="H1" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="C2" s="5">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>8</v>
+      <c r="D2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="F2" s="5">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="5">
-        <v>80</v>
-      </c>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="F3" s="5">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F4" s="5">
+        <v>5</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>66</v>
+      <c r="D5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="F5" s="5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>4</v>
@@ -2557,19 +2564,19 @@
     </row>
     <row r="6" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>25</v>
+      <c r="D6" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="F6" s="5">
         <v>1</v>
@@ -2581,22 +2588,22 @@
     </row>
     <row r="7" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>28</v>
+      <c r="D7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="F7" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>4</v>
@@ -2605,46 +2612,46 @@
     </row>
     <row r="8" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>30</v>
+      <c r="D8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="F8" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="C9" s="5">
         <v>1</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>32</v>
+      <c r="D9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="F9" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>4</v>
@@ -2653,141 +2660,151 @@
     </row>
     <row r="10" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>77</v>
+      <c r="D10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="F10" s="5">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C11" s="5">
         <v>1</v>
       </c>
-      <c r="D11" s="12"/>
+      <c r="D11" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="E11" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F11" s="5">
-        <v>0</v>
-      </c>
-      <c r="G11" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
       </c>
-      <c r="D13" s="12"/>
+      <c r="D13" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="E13" s="5" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="F13" s="5">
-        <v>9</v>
-      </c>
-      <c r="G13" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
       </c>
-      <c r="D14" s="12"/>
+      <c r="D14" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="E14" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F14" s="5">
-        <v>5</v>
-      </c>
-      <c r="G14" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C15" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="F15" s="5">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="5">
-        <v>62</v>
-      </c>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>9</v>
@@ -2796,13 +2813,13 @@
         <v>1</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="F16" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>4</v>
@@ -2811,31 +2828,31 @@
     </row>
     <row r="17" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F17" s="5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>9</v>
@@ -2844,456 +2861,468 @@
         <v>1</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>77</v>
+        <v>40</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="F18" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H18" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="H18" s="5">
+        <v>57</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>66</v>
+      <c r="D19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="F19" s="5">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H19" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="H19" s="5">
+        <v>90</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C20" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="F20" s="5">
         <v>2</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C21" s="5">
-        <v>1</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="E21" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="F21" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="C22" s="5">
         <v>1</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="F22" s="5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" s="5">
         <v>1</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="F23" s="5">
         <v>2</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C24" s="5">
         <v>1</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>42</v>
+      <c r="D24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="F24" s="5">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C25" s="5">
         <v>1</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>42</v>
+      <c r="D25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="F25" s="5">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="5">
-        <v>57</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="C26" s="5">
         <v>1</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="F26" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="C27" s="5">
         <v>1</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="F27" s="5">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H27" s="5">
-        <v>22</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C28" s="5">
         <v>1</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>25</v>
+      <c r="D28" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="F28" s="5">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="H28" s="5">
+        <v>90</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C29" s="5">
         <v>1</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="F29" s="5">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H29" s="5">
-        <v>28</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C30" s="5">
         <v>1</v>
       </c>
-      <c r="D30" s="12"/>
+      <c r="D30" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="E30" s="5" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="F30" s="5">
-        <v>25</v>
-      </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H30" s="5">
+        <v>72</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C31" s="5">
-        <v>1</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>33</v>
+        <v>2</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>55</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="F31" s="5">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C32" s="5">
         <v>1</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="F32" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C33" s="5">
-        <v>1</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="F33" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="C34" s="5">
         <v>1</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>32</v>
+      <c r="D34" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="F34" s="5">
-        <v>0.5</v>
+        <v>8</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="5">
+        <v>1</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" s="5">
         <v>6</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="5">
-        <v>1</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F35" s="5">
-        <v>0.5</v>
-      </c>
       <c r="G35" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36" s="5">
         <v>1</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>44</v>
+      <c r="D36" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="F36" s="5">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H36" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="H36" s="5">
+        <v>22</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>10</v>
@@ -3302,240 +3331,240 @@
         <v>1</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F37" s="5">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C38" s="5">
         <v>1</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>30</v>
+      <c r="D38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="F38" s="5">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H38" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="H38" s="5">
+        <v>73</v>
+      </c>
     </row>
     <row r="39" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C39" s="5">
         <v>1</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F39" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C40" s="5">
         <v>1</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="F40" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C41" s="5">
         <v>1</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="F41" s="5">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H41" s="5">
-        <v>110</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C42" s="5">
         <v>1</v>
       </c>
-      <c r="D42" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>48</v>
+      <c r="D42" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="F42" s="5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C43" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="F43" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="C44" s="5">
         <v>1</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>77</v>
+        <v>26</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="F44" s="5">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="H44" s="5"/>
     </row>
     <row r="45" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C45" s="5">
         <v>1</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>30</v>
+      <c r="D45" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="F45" s="5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H45" s="5"/>
     </row>
     <row r="46" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C46" s="5">
         <v>1</v>
       </c>
       <c r="D46" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E46" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="F46" s="5">
         <v>3</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>11</v>
@@ -3544,918 +3573,916 @@
         <v>1</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F47" s="5">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H47" s="5"/>
     </row>
     <row r="48" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C48" s="5">
         <v>1</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="F48" s="5">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C49" s="5">
         <v>1</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F49" s="5">
         <v>1</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C50" s="5">
         <v>1</v>
       </c>
-      <c r="D50" s="4" t="s">
-        <v>24</v>
+      <c r="D50" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F50" s="5">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H50" s="5"/>
     </row>
     <row r="51" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C51" s="5">
         <v>1</v>
       </c>
       <c r="D51" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E51" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E51" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="F51" s="5">
         <v>1</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H51" s="5"/>
     </row>
     <row r="52" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C52" s="5">
         <v>1</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F52" s="5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="H52" s="5"/>
     </row>
     <row r="53" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C53" s="5">
         <v>1</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F53" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H53" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="H53" s="5">
+        <v>28</v>
+      </c>
     </row>
     <row r="54" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C54" s="5">
         <v>1</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="F54" s="5">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H54" s="5">
-        <v>90</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C55" s="5">
         <v>1</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F55" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C56" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="F56" s="5">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H56" s="5">
-        <v>73</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="H56" s="5"/>
     </row>
     <row r="57" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C57" s="5">
-        <v>1</v>
-      </c>
-      <c r="D57" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E57" s="20" t="s">
-        <v>61</v>
+        <v>2</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>36</v>
       </c>
       <c r="F57" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H57" s="5"/>
     </row>
     <row r="58" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C58" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F58" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H58" s="5"/>
     </row>
     <row r="59" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C59" s="5">
         <v>1</v>
       </c>
-      <c r="D59" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E59" s="11" t="s">
-        <v>77</v>
+      <c r="D59" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="F59" s="5">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="H59" s="5">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C60" s="5">
         <v>1</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="F60" s="5">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H60" s="5"/>
     </row>
     <row r="61" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C61" s="5">
         <v>1</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="F61" s="5">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H61" s="5">
-        <v>75</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C62" s="5">
         <v>1</v>
       </c>
-      <c r="D62" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>23</v>
+      <c r="D62" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>60</v>
       </c>
       <c r="F62" s="5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="H62" s="5"/>
     </row>
     <row r="63" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C63" s="5">
         <v>1</v>
       </c>
-      <c r="D63" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>66</v>
+      <c r="D63" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>60</v>
       </c>
       <c r="F63" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H63" s="5"/>
     </row>
     <row r="64" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C64" s="5">
         <v>1</v>
       </c>
-      <c r="D64" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>77</v>
+      <c r="D64" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>60</v>
       </c>
       <c r="F64" s="5">
         <v>15</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="H64" s="5"/>
     </row>
     <row r="65" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C65" s="5">
-        <v>1</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>30</v>
+        <v>2</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>60</v>
       </c>
       <c r="F65" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H65" s="5"/>
     </row>
     <row r="66" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C66" s="5">
         <v>1</v>
       </c>
-      <c r="D66" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>28</v>
+      <c r="D66" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="F66" s="5">
-        <v>7</v>
+        <v>0.5</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H66" s="5"/>
     </row>
     <row r="67" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C67" s="5">
-        <v>1</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="D67" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="F67" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H67" s="5"/>
     </row>
     <row r="68" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C68" s="5">
-        <v>1</v>
-      </c>
-      <c r="D68" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>51</v>
+        <v>2</v>
+      </c>
+      <c r="D68" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="F68" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H68" s="5"/>
     </row>
     <row r="69" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C69" s="5">
-        <v>1</v>
-      </c>
-      <c r="D69" s="19" t="s">
-        <v>71</v>
+        <v>2</v>
+      </c>
+      <c r="D69" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="E69" s="20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F69" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H69" s="5"/>
     </row>
     <row r="70" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C70" s="5">
         <v>1</v>
       </c>
-      <c r="D70" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>32</v>
+      <c r="D70" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="F70" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H70" s="5"/>
     </row>
     <row r="71" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C71" s="5">
         <v>1</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F71" s="5">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H71" s="5">
-        <v>90</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="H71" s="5"/>
     </row>
     <row r="72" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="C72" s="5">
         <v>1</v>
       </c>
-      <c r="D72" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>8</v>
+      <c r="D72" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="F72" s="5">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H72" s="5">
-        <v>72</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="H72" s="5"/>
     </row>
     <row r="73" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C73" s="5">
         <v>1</v>
       </c>
-      <c r="D73" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E73" s="20" t="s">
-        <v>61</v>
+      <c r="D73" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E73" s="21" t="s">
+        <v>31</v>
       </c>
       <c r="F73" s="5">
-        <v>15</v>
+        <v>0.5</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H73" s="5"/>
     </row>
     <row r="74" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C74" s="5">
         <v>1</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="F74" s="5">
-        <v>7</v>
+        <v>0.5</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H74" s="5"/>
     </row>
     <row r="75" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C75" s="5">
         <v>1</v>
       </c>
-      <c r="D75" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E75" s="11" t="s">
-        <v>77</v>
+      <c r="D75" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="F75" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="H75" s="5"/>
     </row>
     <row r="76" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C76" s="5">
         <v>1</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F76" s="5">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H76" s="5"/>
     </row>
     <row r="77" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C77" s="5">
         <v>1</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F77" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H77" s="5"/>
     </row>
     <row r="78" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C78" s="5">
-        <v>1</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>65</v>
+        <v>2</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>62</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="F78" s="5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H78" s="5"/>
     </row>
     <row r="79" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C79" s="5">
-        <v>1</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>37</v>
+        <v>2</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E79" s="14" t="s">
+        <v>53</v>
       </c>
       <c r="F79" s="5">
-        <v>7</v>
+        <v>0.5</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H79" s="5"/>
     </row>
     <row r="80" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C80" s="5">
-        <v>1</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>32</v>
+        <v>2</v>
+      </c>
+      <c r="D80" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E80" s="14" t="s">
+        <v>53</v>
       </c>
       <c r="F80" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H80" s="5"/>
     </row>
     <row r="81" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C81" s="5">
         <v>1</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="D81" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E81" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E81" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="F81" s="5">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H81" s="5"/>
     </row>
     <row r="82" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C82" s="5">
         <v>1</v>
       </c>
-      <c r="D82" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>26</v>
+      <c r="D82" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E82" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="F82" s="5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H82" s="5"/>
     </row>
     <row r="83" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C83" s="5">
         <v>1</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F83" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H83" s="5"/>
     </row>
     <row r="84" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C84" s="5">
         <v>2</v>
       </c>
-      <c r="D84" s="12"/>
+      <c r="D84" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="E84" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F84" s="5">
-        <v>88</v>
-      </c>
-      <c r="G84" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="H84" s="5"/>
     </row>
     <row r="85" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>14</v>
@@ -4464,70 +4491,70 @@
         <v>2</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F85" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H85" s="5"/>
     </row>
     <row r="86" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C86" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="F86" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H86" s="5"/>
     </row>
     <row r="87" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C87" s="5">
         <v>2</v>
       </c>
       <c r="D87" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F87" s="5">
         <v>1</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H87" s="5"/>
     </row>
     <row r="88" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>14</v>
@@ -4535,472 +4562,467 @@
       <c r="C88" s="5">
         <v>2</v>
       </c>
-      <c r="D88" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E88" s="11" t="s">
+      <c r="D88" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="E88" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="F88" s="5">
-        <v>0.5</v>
+        <v>7</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H88" s="5"/>
     </row>
     <row r="89" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C89" s="5">
         <v>2</v>
       </c>
-      <c r="D89" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E89" s="14" t="s">
-        <v>54</v>
+      <c r="D89" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="F89" s="5">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H89" s="5"/>
     </row>
     <row r="90" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B90" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="C90" s="5">
-        <v>2</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>41</v>
+        <v>1</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="F90" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="H90" s="5"/>
     </row>
     <row r="91" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C91" s="5">
-        <v>2</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="F91" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H91" s="5"/>
     </row>
     <row r="92" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C92" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F92" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H92" s="5"/>
     </row>
     <row r="93" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C93" s="5">
-        <v>2</v>
-      </c>
-      <c r="D93" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E93" s="11" t="s">
-        <v>59</v>
+        <v>1</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="F93" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H93" s="5"/>
     </row>
     <row r="94" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C94" s="5">
-        <v>2</v>
-      </c>
-      <c r="D94" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E94" s="20" t="s">
-        <v>61</v>
+        <v>1</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E94" s="21" t="s">
+        <v>25</v>
       </c>
       <c r="F94" s="5">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H94" s="5"/>
     </row>
     <row r="95" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B95" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="C95" s="5">
-        <v>2</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>38</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D95" s="12"/>
       <c r="E95" s="5" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="F95" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="H95" s="5"/>
     </row>
     <row r="96" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C96" s="5">
-        <v>2</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>43</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D96" s="12"/>
       <c r="E96" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F96" s="5">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="H96" s="5"/>
     </row>
     <row r="97" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C97" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D97" s="12"/>
       <c r="E97" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F97" s="5">
-        <v>70</v>
-      </c>
-      <c r="G97" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="H97" s="5"/>
     </row>
     <row r="98" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C98" s="5">
         <v>2</v>
       </c>
-      <c r="D98" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="D98" s="12"/>
       <c r="E98" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F98" s="5">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="H98" s="5"/>
     </row>
     <row r="99" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C99" s="5">
         <v>2</v>
       </c>
-      <c r="D99" s="4" t="s">
-        <v>41</v>
-      </c>
+      <c r="D99" s="12"/>
       <c r="E99" s="5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F99" s="5">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="H99" s="5"/>
     </row>
     <row r="100" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C100" s="5">
         <v>2</v>
       </c>
-      <c r="D100" s="4" t="s">
+      <c r="D100" s="12"/>
+      <c r="E100" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F100" s="5">
         <v>60</v>
       </c>
-      <c r="E100" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F100" s="5">
-        <v>3</v>
-      </c>
       <c r="G100" s="5" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="H100" s="5"/>
     </row>
     <row r="101" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C101" s="5">
-        <v>2</v>
-      </c>
-      <c r="D101" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E101" s="11" t="s">
-        <v>59</v>
+        <v>1</v>
+      </c>
+      <c r="D101" s="12"/>
+      <c r="E101" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="F101" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="H101" s="5"/>
     </row>
     <row r="102" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B102" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="C102" s="5">
-        <v>2</v>
-      </c>
-      <c r="D102" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E102" s="5" t="s">
-        <v>62</v>
+        <v>1</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E102" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="F102" s="5">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H102" s="5"/>
     </row>
     <row r="103" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C103" s="5">
-        <v>2</v>
-      </c>
-      <c r="D103" s="12"/>
-      <c r="E103" s="5" t="s">
-        <v>35</v>
+        <v>1</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E103" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="F103" s="5">
-        <v>60</v>
-      </c>
-      <c r="G103" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="G103" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="H103" s="5"/>
     </row>
     <row r="104" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C104" s="5">
-        <v>2</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E104" s="5" t="s">
-        <v>37</v>
+        <v>1</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E104" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="F104" s="5">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="H104" s="5"/>
     </row>
     <row r="105" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C105" s="5">
-        <v>2</v>
-      </c>
-      <c r="D105" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E105" s="14" t="s">
-        <v>54</v>
+        <v>1</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E105" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="F105" s="5">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H105" s="5"/>
+        <v>76</v>
+      </c>
+      <c r="H105" s="5">
+        <v>71</v>
+      </c>
     </row>
     <row r="106" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C106" s="5">
-        <v>2</v>
-      </c>
-      <c r="D106" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E106" s="5" t="s">
-        <v>30</v>
+        <v>1</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E106" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="F106" s="5">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G106" s="5" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="H106" s="5"/>
     </row>
     <row r="107" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B107" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C107" s="17">
-        <v>2</v>
-      </c>
-      <c r="D107" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E107" s="17" t="s">
-        <v>55</v>
+        <v>1</v>
+      </c>
+      <c r="D107" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E107" s="23" t="s">
+        <v>75</v>
       </c>
       <c r="F107" s="17">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G107" s="17" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="H107" s="17"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:IN107">
-    <sortCondition ref="C2:C107"/>
-    <sortCondition ref="B2:B107"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H107">
+    <sortCondition ref="G2:G107"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>